<commit_message>
Test 3 prep minor update number 4
New R files for installation and creating forms and letters
</commit_message>
<xml_diff>
--- a/NRCS_Wetland_Tools_Pro/SUPPORT/Templates/NRCS_Address.xlsx
+++ b/NRCS_Wetland_Tools_Pro/SUPPORT/Templates/NRCS_Address.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIS_Tools\python_scripts\GitHub\Wetland_Tools_Pro\NRCS_Wetland_Tools_Pro\SUPPORT\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIS_Tools\NRCS_Wetland_Tools_Pro\SUPPORT\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81B41D21-41A4-4047-8437-E7600FF0C28E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1EB3896-5AA0-4A2B-919E-A6EDE93B8FF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12900" yWindow="4440" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -482,7 +482,7 @@
   <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>